<commit_message>
This is a new commit for what I originally planned to be amended
</commit_message>
<xml_diff>
--- a/public/file/customer/coba.xlsx
+++ b/public/file/customer/coba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECBB4AB-D66E-6E48-9476-00E5D4B5EE49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1DC435-E6E8-FE4F-8307-35BA65EE50A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{65889EF1-B67D-1F47-95EA-1299CB4AA74D}"/>
   </bookViews>
@@ -397,19 +397,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57ADFC99-F279-784E-81BD-87BA3AB56C0F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -419,11 +420,11 @@
       <c r="C1">
         <v>324</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -433,11 +434,11 @@
       <c r="C2">
         <v>3423</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -447,11 +448,11 @@
       <c r="C3">
         <v>89939948</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -461,11 +462,11 @@
       <c r="C4">
         <v>980</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -475,11 +476,11 @@
       <c r="C5">
         <v>9898</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -489,7 +490,7 @@
       <c r="C6">
         <v>8989867654</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>